<commit_message>
Nova correcao de pvs
</commit_message>
<xml_diff>
--- a/PVs/parede.xlsx
+++ b/PVs/parede.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonardo.leao\Desktop\Concrete-Instrum-Scripts\PVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68927AB8-67A5-450D-BB10-CA44B8EA68F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06E8619-0F97-48CD-9586-6B98356A2740}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="1455" windowWidth="21600" windowHeight="11400" xr2:uid="{8C664926-5403-41C4-B638-B597EA4F600E}"/>
+    <workbookView xWindow="3000" yWindow="3000" windowWidth="21600" windowHeight="11400" xr2:uid="{8C664926-5403-41C4-B638-B597EA4F600E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="40">
   <si>
     <t>Localização</t>
   </si>
@@ -122,37 +122,7 @@
     <t>L2L3</t>
   </si>
   <si>
-    <t>L2L4</t>
-  </si>
-  <si>
-    <t>L2L5</t>
-  </si>
-  <si>
-    <t>L2L6</t>
-  </si>
-  <si>
-    <t>L2L7</t>
-  </si>
-  <si>
-    <t>L2L8</t>
-  </si>
-  <si>
-    <t>L2L9</t>
-  </si>
-  <si>
-    <t>L2L10</t>
-  </si>
-  <si>
     <t>L6P8</t>
-  </si>
-  <si>
-    <t>L6P9</t>
-  </si>
-  <si>
-    <t>L6P10</t>
-  </si>
-  <si>
-    <t>L6P11</t>
   </si>
   <si>
     <t>H_Hx</t>
@@ -189,10 +159,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -546,7 +522,7 @@
   <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +555,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3">
         <v>22</v>
@@ -593,7 +569,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C3" s="3">
         <v>22</v>
@@ -615,7 +591,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3">
         <v>25</v>
@@ -626,7 +602,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="3">
         <v>25</v>
@@ -637,7 +613,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="3">
         <v>25</v>
@@ -648,7 +624,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C8" s="3">
         <v>25</v>
@@ -659,7 +635,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3">
         <v>25</v>
@@ -670,7 +646,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3">
         <v>25</v>
@@ -681,7 +657,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3">
         <v>25</v>
@@ -695,7 +671,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3">
         <v>26</v>
@@ -709,7 +685,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3">
         <v>26</v>
@@ -720,7 +696,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C14" s="3">
         <v>26</v>
@@ -731,7 +707,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C15" s="3">
         <v>26</v>
@@ -742,7 +718,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C16" s="3">
         <v>26</v>
@@ -753,7 +729,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3">
         <v>26</v>
@@ -795,7 +771,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C20" s="3">
         <v>18</v>
@@ -809,7 +785,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C21" s="3">
         <v>18</v>
@@ -837,7 +813,7 @@
         <v>11</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C23" s="3">
         <v>18</v>
@@ -851,7 +827,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3">
         <v>18</v>
@@ -949,7 +925,7 @@
         <v>19</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C31" s="3">
         <v>21</v>
@@ -963,7 +939,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C32" s="3">
         <v>21</v>
@@ -977,7 +953,7 @@
         <v>19</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C33" s="3">
         <v>21</v>
@@ -991,7 +967,7 @@
         <v>19</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C34" s="3">
         <v>21</v>
@@ -1019,7 +995,7 @@
         <v>19</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C36" s="3">
         <v>21</v>
@@ -1033,7 +1009,7 @@
         <v>19</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C37" s="3">
         <v>21</v>
@@ -1047,7 +1023,7 @@
         <v>19</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C38" s="3">
         <v>26</v>
@@ -1061,7 +1037,7 @@
         <v>19</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C39" s="3">
         <v>26</v>
@@ -1089,7 +1065,7 @@
         <v>21</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C41" s="3">
         <v>21</v>
@@ -1103,7 +1079,7 @@
         <v>21</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C42" s="3">
         <v>21</v>
@@ -1117,7 +1093,7 @@
         <v>21</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C43" s="3">
         <v>21</v>
@@ -1131,7 +1107,7 @@
         <v>21</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C44" s="3">
         <v>21</v>
@@ -1159,7 +1135,7 @@
         <v>21</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C46" s="3">
         <v>21</v>
@@ -1173,7 +1149,7 @@
         <v>21</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C47" s="3">
         <v>21</v>
@@ -1201,7 +1177,7 @@
         <v>22</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C49" s="3">
         <v>19</v>
@@ -1215,7 +1191,7 @@
         <v>22</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C50" s="3">
         <v>19</v>
@@ -1229,7 +1205,7 @@
         <v>22</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C51" s="3">
         <v>19</v>
@@ -1243,7 +1219,7 @@
         <v>22</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C52" s="3">
         <v>19</v>
@@ -1257,7 +1233,7 @@
         <v>22</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C53" s="3">
         <v>19</v>
@@ -1271,7 +1247,7 @@
         <v>22</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C54" s="3">
         <v>19</v>
@@ -1285,7 +1261,7 @@
         <v>22</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C55" s="3">
         <v>20</v>
@@ -1299,7 +1275,7 @@
         <v>22</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C56" s="3">
         <v>20</v>
@@ -1327,7 +1303,7 @@
         <v>24</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C58" s="3">
         <v>19</v>
@@ -1341,7 +1317,7 @@
         <v>24</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C59" s="3">
         <v>19</v>
@@ -1355,7 +1331,7 @@
         <v>24</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C60" s="3">
         <v>19</v>
@@ -1369,7 +1345,7 @@
         <v>24</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C61" s="3">
         <v>19</v>
@@ -1397,7 +1373,7 @@
         <v>24</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C63" s="3">
         <v>19</v>
@@ -1411,7 +1387,7 @@
         <v>24</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C64" s="3">
         <v>18</v>
@@ -1425,7 +1401,7 @@
         <v>24</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C65" s="3">
         <v>20</v>
@@ -1439,7 +1415,7 @@
         <v>24</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C66" s="3">
         <v>20</v>
@@ -1491,6 +1467,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>